<commit_message>
added function to upload parcelles
</commit_message>
<xml_diff>
--- a/instance/uploads/stim.xlsx
+++ b/instance/uploads/stim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A8892A-C576-4E03-B1A4-0AF72E73793D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66F8134-4BA1-40DC-865B-607122CD2FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{FE9D42A5-F897-4C6C-9F31-14EABD70FDF1}"/>
   </bookViews>
@@ -25,142 +25,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
-  <si>
-    <t>FSV-0001</t>
-  </si>
-  <si>
-    <t>VAONIRINA</t>
-  </si>
-  <si>
-    <t>ELIA B</t>
-  </si>
-  <si>
-    <t>LAF</t>
-  </si>
-  <si>
-    <t>MAHANARA</t>
-  </si>
-  <si>
-    <t>FSV-0002</t>
-  </si>
-  <si>
-    <t>ZAMANJAZA</t>
-  </si>
-  <si>
-    <t>MAX LADIO</t>
-  </si>
-  <si>
-    <t>FSV</t>
-  </si>
-  <si>
-    <t>SARAHANDRANO</t>
-  </si>
-  <si>
-    <t>FSV-0003</t>
-  </si>
-  <si>
-    <t>RAZAFINDAZA</t>
-  </si>
-  <si>
-    <t>RABENEL MAHAZAKA</t>
-  </si>
-  <si>
-    <t>FSV-0004</t>
-  </si>
-  <si>
-    <t>RAZANAJATOVO</t>
-  </si>
-  <si>
-    <t>FREDERIC</t>
-  </si>
-  <si>
-    <t>FSV-0005</t>
-  </si>
-  <si>
-    <t>ANONDAHY</t>
-  </si>
-  <si>
-    <t>CLERMONT</t>
-  </si>
-  <si>
-    <t>FSV-0006</t>
-  </si>
-  <si>
-    <t>FRANCISA</t>
-  </si>
-  <si>
-    <t>BEO</t>
-  </si>
-  <si>
-    <t>stamp</t>
-  </si>
-  <si>
-    <t>picture</t>
-  </si>
-  <si>
-    <t>idNumber</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>idNumberPicture</t>
-  </si>
-  <si>
-    <t>birthdate</t>
-  </si>
-  <si>
-    <t>inCollaboration</t>
-  </si>
-  <si>
-    <t>nonCollaboarationReason</t>
-  </si>
-  <si>
-    <t>certification</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>grpMembership</t>
-  </si>
-  <si>
-    <t>groupementId</t>
-  </si>
-  <si>
-    <t>villageId</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>vsv-1</t>
-  </si>
-  <si>
-    <t>vsv-2</t>
-  </si>
-  <si>
-    <t>vsv-3</t>
-  </si>
-  <si>
-    <t>vsv-4</t>
-  </si>
-  <si>
-    <t>vsv-5</t>
-  </si>
-  <si>
-    <t>vsv-6</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>plants</t>
+  </si>
+  <si>
+    <t>Plants Productive</t>
+  </si>
+  <si>
+    <t>Age Moyen</t>
+  </si>
+  <si>
+    <t>Production estimee</t>
+  </si>
+  <si>
+    <t>Production estimee vrac</t>
+  </si>
+  <si>
+    <t>inspected</t>
+  </si>
+  <si>
+    <t>Antohaka</t>
+  </si>
+  <si>
+    <t>Tegnarano</t>
+  </si>
+  <si>
+    <t>0.97 Ha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +98,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -249,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -263,6 +177,12 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -578,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC725029-1325-43D3-8A29-C5B1D64E8485}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,10 +509,10 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
@@ -602,250 +522,119 @@
     <col min="15" max="15" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2500</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6</v>
+      </c>
+      <c r="G2" s="7">
+        <v>700</v>
+      </c>
+      <c r="H2" s="8">
+        <v>175</v>
+      </c>
+      <c r="I2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="5">
-        <v>2</v>
-      </c>
-      <c r="I2" s="5">
-        <v>3</v>
-      </c>
-      <c r="K2" s="6">
-        <v>26299</v>
-      </c>
-      <c r="L2" t="b">
-        <v>0</v>
-      </c>
+      <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="3" spans="1:11" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="5">
-        <v>2</v>
-      </c>
-      <c r="I3" s="5">
-        <v>3</v>
-      </c>
-      <c r="K3" s="6">
-        <v>26300</v>
-      </c>
-      <c r="L3" t="b">
-        <v>0</v>
-      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:15" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="4" spans="1:11" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="5">
-        <v>2</v>
-      </c>
-      <c r="I4" s="5">
-        <v>3</v>
-      </c>
-      <c r="K4" s="6">
-        <v>26301</v>
-      </c>
-      <c r="L4" t="b">
-        <v>0</v>
-      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="5" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="5">
-        <v>2</v>
-      </c>
-      <c r="I5" s="5">
-        <v>3</v>
-      </c>
-      <c r="K5" s="6">
-        <v>26302</v>
-      </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="6" spans="1:11" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="5">
-        <v>2</v>
-      </c>
-      <c r="I6" s="5">
-        <v>3</v>
-      </c>
-      <c r="K6" s="6">
-        <v>26303</v>
-      </c>
-      <c r="L6" t="b">
-        <v>0</v>
-      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
-      </c>
+    <row r="7" spans="1:11" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="5">
-        <v>2</v>
-      </c>
-      <c r="I7" s="5">
-        <v>3</v>
-      </c>
-      <c r="K7" s="6">
-        <v>26304</v>
-      </c>
-      <c r="L7" t="b">
-        <v>0</v>
-      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="K7" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>